<commit_message>
formatting correction in task list
</commit_message>
<xml_diff>
--- a/docs/Data Cleanup Procedure Breakdown.xlsx
+++ b/docs/Data Cleanup Procedure Breakdown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391455E5-C249-E044-81A5-1D8271C37B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C045AA6-DE53-9B4E-A270-01FB22E8B171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38260" yWindow="12720" windowWidth="29320" windowHeight="23740" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
+    <workbookView xWindow="38260" yWindow="12720" windowWidth="35460" windowHeight="25180" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="480">
   <si>
     <t xml:space="preserve">[1] "Respondent ID"                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
   </si>
@@ -1473,6 +1473,9 @@
   </si>
   <si>
     <t>[63] - [72]</t>
+  </si>
+  <si>
+    <t>2019 Map</t>
   </si>
 </sst>
 </file>
@@ -1829,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7FEF52-89A2-2F42-A286-59280B1D433F}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1874,7 +1877,7 @@
         <v>355</v>
       </c>
       <c r="H2" t="s">
-        <v>374</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Formattign to make task list a little more readable
</commit_message>
<xml_diff>
--- a/docs/Data Cleanup Procedure Breakdown.xlsx
+++ b/docs/Data Cleanup Procedure Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC6B677-1D91-6F42-86CE-85DC8084B7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9B2DAB-557A-D643-AA94-4184DA158695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="3020" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
+    <workbookView xWindow="2020" yWindow="2660" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="1" r:id="rId1"/>
@@ -1617,7 +1617,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1631,19 +1631,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1652,10 +1689,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1973,51 +2032,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7FEF52-89A2-2F42-A286-59280B1D433F}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="C57" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.6640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="45.6640625" customWidth="1"/>
+    <col min="2" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="70.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.83203125" customWidth="1"/>
     <col min="8" max="8" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5">
         <v>2019</v>
       </c>
-      <c r="E1" s="1">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="9">
         <v>2023</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>478</v>
       </c>
     </row>
@@ -2031,7 +2097,7 @@
       <c r="C3" t="s">
         <v>356</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -2057,7 +2123,7 @@
       <c r="C4" t="s">
         <v>356</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -2083,7 +2149,7 @@
       <c r="C5" t="s">
         <v>356</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2109,7 +2175,7 @@
       <c r="C6" t="s">
         <v>356</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2135,7 +2201,7 @@
       <c r="C7" t="s">
         <v>356</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2161,7 +2227,7 @@
       <c r="C8" t="s">
         <v>356</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>445</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2187,7 +2253,7 @@
       <c r="C9" t="s">
         <v>356</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>446</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2213,7 +2279,7 @@
       <c r="C10" t="s">
         <v>356</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>446</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2239,7 +2305,7 @@
       <c r="C11" t="s">
         <v>356</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2265,7 +2331,7 @@
       <c r="C12" t="s">
         <v>367</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>375</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2291,7 +2357,7 @@
       <c r="C13" t="s">
         <v>369</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>376</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2317,7 +2383,7 @@
       <c r="C14" t="s">
         <v>356</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2343,7 +2409,7 @@
       <c r="C15" t="s">
         <v>356</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2369,7 +2435,7 @@
       <c r="C16" t="s">
         <v>356</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2395,7 +2461,7 @@
       <c r="C17" t="s">
         <v>356</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2421,7 +2487,7 @@
       <c r="C18" t="s">
         <v>356</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2447,7 +2513,7 @@
       <c r="C19" t="s">
         <v>356</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2473,7 +2539,7 @@
       <c r="C20" t="s">
         <v>356</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2499,7 +2565,7 @@
       <c r="C21" t="s">
         <v>356</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2525,7 +2591,7 @@
       <c r="C22" t="s">
         <v>356</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2551,7 +2617,7 @@
       <c r="C23" t="s">
         <v>356</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2577,7 +2643,7 @@
       <c r="C24" t="s">
         <v>356</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2603,7 +2669,7 @@
       <c r="C25" t="s">
         <v>356</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -2629,7 +2695,7 @@
       <c r="C26" t="s">
         <v>356</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2655,7 +2721,7 @@
       <c r="C27" t="s">
         <v>356</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2681,7 +2747,7 @@
       <c r="C28" t="s">
         <v>356</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2707,7 +2773,7 @@
       <c r="C29" t="s">
         <v>356</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -2733,7 +2799,7 @@
       <c r="C30" t="s">
         <v>356</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -2759,7 +2825,7 @@
       <c r="C31" t="s">
         <v>356</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2785,7 +2851,7 @@
       <c r="C32" t="s">
         <v>356</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -2811,7 +2877,7 @@
       <c r="C33" t="s">
         <v>356</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -2837,7 +2903,7 @@
       <c r="C34" t="s">
         <v>356</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -2863,7 +2929,7 @@
       <c r="C35" t="s">
         <v>356</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2889,7 +2955,7 @@
       <c r="C36" t="s">
         <v>356</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -2915,7 +2981,7 @@
       <c r="C37" t="s">
         <v>356</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -2941,7 +3007,7 @@
       <c r="C38" t="s">
         <v>356</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -2967,7 +3033,7 @@
       <c r="C39" t="s">
         <v>356</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -2993,7 +3059,7 @@
       <c r="C40" t="s">
         <v>356</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -3019,7 +3085,7 @@
       <c r="C41" t="s">
         <v>356</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3045,7 +3111,7 @@
       <c r="C42" t="s">
         <v>356</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3071,7 +3137,7 @@
       <c r="C43" t="s">
         <v>356</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -3097,7 +3163,7 @@
       <c r="C44" t="s">
         <v>356</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -3123,7 +3189,7 @@
       <c r="C45" t="s">
         <v>356</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3149,7 +3215,7 @@
       <c r="C46" t="s">
         <v>356</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3175,7 +3241,7 @@
       <c r="C47" t="s">
         <v>356</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3201,7 +3267,7 @@
       <c r="C48" t="s">
         <v>356</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3227,7 +3293,7 @@
       <c r="C49" t="s">
         <v>356</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -3253,7 +3319,7 @@
       <c r="C50" t="s">
         <v>356</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3279,7 +3345,7 @@
       <c r="C51" t="s">
         <v>367</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="7" t="s">
         <v>450</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -3305,7 +3371,7 @@
       <c r="C52" t="s">
         <v>384</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="7" t="s">
         <v>388</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -3331,7 +3397,7 @@
       <c r="C53" t="s">
         <v>385</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="7" t="s">
         <v>388</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -3357,7 +3423,7 @@
       <c r="C54" t="s">
         <v>390</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="7" t="s">
         <v>389</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -3383,7 +3449,7 @@
       <c r="C55" t="s">
         <v>390</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="7" t="s">
         <v>389</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -3409,7 +3475,7 @@
       <c r="C56" t="s">
         <v>392</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -3435,7 +3501,7 @@
       <c r="C57" t="s">
         <v>392</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -3461,7 +3527,7 @@
       <c r="C58" t="s">
         <v>392</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -3487,7 +3553,7 @@
       <c r="C59" t="s">
         <v>392</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -3513,7 +3579,7 @@
       <c r="C60" t="s">
         <v>392</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -3539,7 +3605,7 @@
       <c r="C61" t="s">
         <v>392</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -3565,7 +3631,7 @@
       <c r="C62" t="s">
         <v>392</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -3591,7 +3657,7 @@
       <c r="C63" t="s">
         <v>392</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -3617,7 +3683,7 @@
       <c r="C64" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="7" t="s">
         <v>472</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -3643,7 +3709,7 @@
       <c r="C65" t="s">
         <v>392</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -3669,7 +3735,7 @@
       <c r="C66" t="s">
         <v>392</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -3695,7 +3761,7 @@
       <c r="C67" t="s">
         <v>392</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -3715,7 +3781,7 @@
       <c r="C68" t="s">
         <v>392</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -3735,7 +3801,7 @@
       <c r="C69" t="s">
         <v>392</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E69" s="1" t="s">
@@ -3755,7 +3821,7 @@
       <c r="C70" t="s">
         <v>392</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E70" s="1" t="s">
@@ -3775,7 +3841,7 @@
       <c r="C71" t="s">
         <v>392</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -3795,7 +3861,7 @@
       <c r="C72" t="s">
         <v>392</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -3815,7 +3881,7 @@
       <c r="C73" t="s">
         <v>356</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -3835,7 +3901,7 @@
       <c r="C74" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="7" t="s">
         <v>476</v>
       </c>
       <c r="E74" s="1" t="s">
@@ -3855,7 +3921,7 @@
       <c r="C75" t="s">
         <v>367</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="7" t="s">
         <v>483</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -3875,7 +3941,7 @@
       <c r="C76" t="s">
         <v>484</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E76" s="1" t="s">
@@ -3895,7 +3961,7 @@
       <c r="C77" t="s">
         <v>485</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="7" t="s">
         <v>482</v>
       </c>
       <c r="E77" s="1" t="s">
@@ -3915,7 +3981,7 @@
       <c r="C78" t="s">
         <v>406</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E78" s="1" t="s">
@@ -3935,7 +4001,7 @@
       <c r="C79" t="s">
         <v>406</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E79" s="1" t="s">
@@ -3955,7 +4021,7 @@
       <c r="C80" t="s">
         <v>406</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -3975,7 +4041,7 @@
       <c r="C81" t="s">
         <v>406</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E81" s="1" t="s">
@@ -3995,7 +4061,7 @@
       <c r="C82" t="s">
         <v>406</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -4015,7 +4081,7 @@
       <c r="C83" t="s">
         <v>406</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="7" t="s">
         <v>489</v>
       </c>
       <c r="E83" s="1" t="s">
@@ -4035,7 +4101,7 @@
       <c r="C84" t="s">
         <v>407</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="7" t="s">
         <v>498</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -4055,7 +4121,7 @@
       <c r="C85" t="s">
         <v>407</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="7" t="s">
         <v>498</v>
       </c>
       <c r="E85" s="1" t="s">
@@ -4075,7 +4141,7 @@
       <c r="C86" t="s">
         <v>407</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="7" t="s">
         <v>498</v>
       </c>
       <c r="E86" s="1" t="s">
@@ -4095,7 +4161,7 @@
       <c r="C87" t="s">
         <v>356</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="7" t="s">
         <v>499</v>
       </c>
       <c r="E87" s="1" t="s">
@@ -4115,7 +4181,7 @@
       <c r="C88" t="s">
         <v>367</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E88" s="1" t="s">
@@ -4135,7 +4201,7 @@
       <c r="C89" t="s">
         <v>356</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -4155,7 +4221,7 @@
       <c r="C90" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="8" t="s">
         <v>503</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -4175,7 +4241,7 @@
       <c r="C91" t="s">
         <v>356</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="8" t="s">
         <v>503</v>
       </c>
       <c r="E91" s="1" t="s">
@@ -4195,7 +4261,7 @@
       <c r="C92" t="s">
         <v>367</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -4215,7 +4281,7 @@
       <c r="C93" t="s">
         <v>356</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E93" s="1" t="s">
@@ -4235,7 +4301,7 @@
       <c r="C94" t="s">
         <v>419</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E94" s="1" t="s">
@@ -4255,7 +4321,7 @@
       <c r="C95" t="s">
         <v>419</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E95" s="1" t="s">
@@ -4275,7 +4341,7 @@
       <c r="C96" t="s">
         <v>419</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -4295,7 +4361,7 @@
       <c r="C97" t="s">
         <v>419</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E97" s="1" t="s">
@@ -4315,7 +4381,7 @@
       <c r="C98" t="s">
         <v>419</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -4335,7 +4401,7 @@
       <c r="C99" t="s">
         <v>419</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -4355,7 +4421,7 @@
       <c r="C100" t="s">
         <v>419</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E100" s="1" t="s">
@@ -4375,7 +4441,7 @@
       <c r="C101" t="s">
         <v>419</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -4395,7 +4461,7 @@
       <c r="C102" t="s">
         <v>419</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E102" s="1" t="s">
@@ -4415,7 +4481,7 @@
       <c r="C103" t="s">
         <v>356</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -4435,7 +4501,7 @@
       <c r="C104" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E104" s="1" t="s">
@@ -4455,7 +4521,7 @@
       <c r="C105" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -4475,7 +4541,7 @@
       <c r="C106" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E106" s="1" t="s">
@@ -4495,7 +4561,7 @@
       <c r="C107" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E107" s="1" t="s">
@@ -4515,7 +4581,7 @@
       <c r="C108" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -4535,7 +4601,7 @@
       <c r="C109" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E109" s="1" t="s">
@@ -4555,7 +4621,7 @@
       <c r="C110" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E110" s="1" t="s">
@@ -4575,7 +4641,7 @@
       <c r="C111" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -4595,7 +4661,7 @@
       <c r="C112" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -4615,7 +4681,7 @@
       <c r="C113" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E113" s="1" t="s">
@@ -4635,7 +4701,7 @@
       <c r="C114" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="7" t="s">
         <v>438</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -4655,7 +4721,7 @@
       <c r="C115" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E115" s="1" t="s">
@@ -4675,7 +4741,7 @@
       <c r="C116" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -4695,7 +4761,7 @@
       <c r="C117" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E117" s="1" t="s">
@@ -4715,7 +4781,7 @@
       <c r="C118" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -4735,7 +4801,7 @@
       <c r="C119" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -4755,7 +4821,7 @@
       <c r="C120" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -4775,7 +4841,7 @@
       <c r="C121" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E121" s="1" t="s">
@@ -4795,7 +4861,7 @@
       <c r="C122" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -4815,7 +4881,7 @@
       <c r="C123" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -4835,7 +4901,7 @@
       <c r="C124" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -4855,7 +4921,7 @@
       <c r="C125" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -4875,7 +4941,7 @@
       <c r="C126" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="8" t="s">
         <v>507</v>
       </c>
       <c r="E126" s="1" t="s">
@@ -4895,7 +4961,7 @@
       <c r="C127" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4909,7 +4975,7 @@
       <c r="C128" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4923,7 +4989,7 @@
       <c r="C129" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4937,7 +5003,7 @@
       <c r="C130" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4951,7 +5017,7 @@
       <c r="C131" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4965,7 +5031,7 @@
       <c r="C132" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4979,7 +5045,7 @@
       <c r="C133" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4993,7 +5059,7 @@
       <c r="C134" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5007,7 +5073,7 @@
       <c r="C135" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D135" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5021,7 +5087,7 @@
       <c r="C136" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="D136" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5035,7 +5101,7 @@
       <c r="C137" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5049,7 +5115,7 @@
       <c r="C138" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D138" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5063,7 +5129,7 @@
       <c r="C139" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D139" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5077,7 +5143,7 @@
       <c r="C140" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D140" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5091,7 +5157,7 @@
       <c r="C141" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D141" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5105,7 +5171,7 @@
       <c r="C142" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D142" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5119,7 +5185,7 @@
       <c r="C143" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D143" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5133,7 +5199,7 @@
       <c r="C144" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D144" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5147,7 +5213,7 @@
       <c r="C145" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D145" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5161,7 +5227,7 @@
       <c r="C146" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D146" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5175,7 +5241,7 @@
       <c r="C147" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D147" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5189,7 +5255,7 @@
       <c r="C148" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="D148" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5203,7 +5269,7 @@
       <c r="C149" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D149" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5217,7 +5283,7 @@
       <c r="C150" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="D150" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5231,7 +5297,7 @@
       <c r="C151" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="D151" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5245,7 +5311,7 @@
       <c r="C152" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="D152" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5259,7 +5325,7 @@
       <c r="C153" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="D153" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5273,7 +5339,7 @@
       <c r="C154" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D154" s="1" t="s">
+      <c r="D154" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5287,7 +5353,7 @@
       <c r="C155" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="D155" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5301,7 +5367,7 @@
       <c r="C156" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D156" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5315,7 +5381,7 @@
       <c r="C157" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D157" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5329,7 +5395,7 @@
       <c r="C158" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="D158" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5343,7 +5409,7 @@
       <c r="C159" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="D159" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5357,7 +5423,7 @@
       <c r="C160" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="D160" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5371,7 +5437,7 @@
       <c r="C161" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="D161" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5385,7 +5451,7 @@
       <c r="C162" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D162" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5399,7 +5465,7 @@
       <c r="C163" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D163" s="1" t="s">
+      <c r="D163" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5413,7 +5479,7 @@
       <c r="C164" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D164" s="1" t="s">
+      <c r="D164" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5427,7 +5493,7 @@
       <c r="C165" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="D165" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5441,7 +5507,7 @@
       <c r="C166" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="D166" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5455,7 +5521,7 @@
       <c r="C167" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="D167" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5469,7 +5535,7 @@
       <c r="C168" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D168" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5483,7 +5549,7 @@
       <c r="C169" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="D169" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5497,7 +5563,7 @@
       <c r="C170" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="D170" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5511,7 +5577,7 @@
       <c r="C171" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="D171" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5525,7 +5591,7 @@
       <c r="C172" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D172" s="1" t="s">
+      <c r="D172" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5539,7 +5605,7 @@
       <c r="C173" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D173" s="1" t="s">
+      <c r="D173" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5553,7 +5619,7 @@
       <c r="C174" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D174" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5567,7 +5633,7 @@
       <c r="C175" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="D175" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5581,7 +5647,7 @@
       <c r="C176" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D176" s="1" t="s">
+      <c r="D176" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5595,7 +5661,7 @@
       <c r="C177" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D177" s="1" t="s">
+      <c r="D177" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5609,7 +5675,7 @@
       <c r="C178" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D178" s="1" t="s">
+      <c r="D178" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5623,7 +5689,7 @@
       <c r="C179" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D179" s="1" t="s">
+      <c r="D179" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5637,7 +5703,7 @@
       <c r="C180" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D180" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5651,7 +5717,7 @@
       <c r="C181" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="D181" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5665,7 +5731,7 @@
       <c r="C182" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D182" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5679,7 +5745,7 @@
       <c r="C183" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="D183" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5693,7 +5759,7 @@
       <c r="C184" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D184" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5707,7 +5773,7 @@
       <c r="C185" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D185" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5721,7 +5787,7 @@
       <c r="C186" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="D186" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5735,7 +5801,7 @@
       <c r="C187" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="D187" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5749,7 +5815,7 @@
       <c r="C188" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D188" s="1" t="s">
+      <c r="D188" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5763,7 +5829,7 @@
       <c r="C189" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D189" s="1" t="s">
+      <c r="D189" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5777,7 +5843,7 @@
       <c r="C190" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D190" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5791,7 +5857,7 @@
       <c r="C191" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D191" s="1" t="s">
+      <c r="D191" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5805,7 +5871,7 @@
       <c r="C192" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D192" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5819,7 +5885,7 @@
       <c r="C193" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D193" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5833,7 +5899,7 @@
       <c r="C194" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D194" s="1" t="s">
+      <c r="D194" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5847,7 +5913,7 @@
       <c r="C195" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="D195" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5861,7 +5927,7 @@
       <c r="C196" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="D196" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5875,7 +5941,7 @@
       <c r="C197" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D197" s="1" t="s">
+      <c r="D197" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5889,7 +5955,7 @@
       <c r="C198" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D198" s="1" t="s">
+      <c r="D198" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5903,7 +5969,7 @@
       <c r="C199" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D199" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5917,7 +5983,7 @@
       <c r="C200" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D200" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5931,7 +5997,7 @@
       <c r="C201" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="D201" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5945,7 +6011,7 @@
       <c r="C202" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="D202" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5959,7 +6025,7 @@
       <c r="C203" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D203" s="1" t="s">
+      <c r="D203" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5973,7 +6039,7 @@
       <c r="C204" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="D204" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5987,7 +6053,7 @@
       <c r="C205" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D205" s="1" t="s">
+      <c r="D205" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6001,7 +6067,7 @@
       <c r="C206" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D206" s="1" t="s">
+      <c r="D206" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6015,7 +6081,7 @@
       <c r="C207" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D207" s="1" t="s">
+      <c r="D207" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6029,7 +6095,7 @@
       <c r="C208" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D208" s="1" t="s">
+      <c r="D208" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6043,7 +6109,7 @@
       <c r="C209" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D209" s="1" t="s">
+      <c r="D209" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6057,7 +6123,7 @@
       <c r="C210" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D210" s="1" t="s">
+      <c r="D210" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6071,7 +6137,7 @@
       <c r="C211" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D211" s="1" t="s">
+      <c r="D211" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6085,7 +6151,7 @@
       <c r="C212" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D212" s="1" t="s">
+      <c r="D212" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6099,7 +6165,7 @@
       <c r="C213" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D213" s="1" t="s">
+      <c r="D213" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6113,7 +6179,7 @@
       <c r="C214" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D214" s="1" t="s">
+      <c r="D214" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6127,7 +6193,7 @@
       <c r="C215" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D215" s="1" t="s">
+      <c r="D215" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6141,7 +6207,7 @@
       <c r="C216" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D216" s="1" t="s">
+      <c r="D216" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6155,7 +6221,7 @@
       <c r="C217" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D217" s="1" t="s">
+      <c r="D217" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6169,7 +6235,7 @@
       <c r="C218" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D218" s="1" t="s">
+      <c r="D218" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6183,7 +6249,7 @@
       <c r="C219" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="D219" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6197,7 +6263,7 @@
       <c r="C220" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D220" s="1" t="s">
+      <c r="D220" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6211,7 +6277,7 @@
       <c r="C221" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="D221" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6225,7 +6291,7 @@
       <c r="C222" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D222" s="1" t="s">
+      <c r="D222" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6239,7 +6305,7 @@
       <c r="C223" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D223" s="1" t="s">
+      <c r="D223" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6253,7 +6319,7 @@
       <c r="C224" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D224" s="1" t="s">
+      <c r="D224" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6267,7 +6333,7 @@
       <c r="C225" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D225" s="1" t="s">
+      <c r="D225" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6281,7 +6347,7 @@
       <c r="C226" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D226" s="1" t="s">
+      <c r="D226" s="8" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6295,7 +6361,7 @@
       <c r="C227" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D227" s="1" t="s">
+      <c r="D227" s="8" t="s">
         <v>511</v>
       </c>
     </row>
@@ -6309,7 +6375,7 @@
       <c r="C228" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D228" s="1" t="s">
+      <c r="D228" s="8" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6323,7 +6389,7 @@
       <c r="C229" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="D229" s="1" t="s">
+      <c r="D229" s="8" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6337,11 +6403,15 @@
       <c r="C230" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D230" s="1" t="s">
+      <c r="D230" s="8" t="s">
         <v>438</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data cleaning task list finished
</commit_message>
<xml_diff>
--- a/docs/Data Cleanup Procedure Breakdown.xlsx
+++ b/docs/Data Cleanup Procedure Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A0E0F2-CD14-FA43-B758-F43863DF712E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72D7B8A-C7F7-864A-AAF7-ABF9B57D9F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2300" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
+    <workbookView xWindow="14020" yWindow="7240" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="575">
   <si>
     <t xml:space="preserve">[1] "Respondent ID"                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
   </si>
@@ -1611,6 +1611,156 @@
   </si>
   <si>
     <t>Open comment for level of involvement, lots of useful feedback and added detail but redundant for analysis</t>
+  </si>
+  <si>
+    <t>Yes/No for collaboration with other H2H members</t>
+  </si>
+  <si>
+    <t>Yes/No for a formal collaboration</t>
+  </si>
+  <si>
+    <t>Yes/no for an informal collaboration</t>
+  </si>
+  <si>
+    <t>Open response for contet on 65-67 above, varied interpretations. Some just list names of orgs, others describe type of work.</t>
+  </si>
+  <si>
+    <t>Check for if H2H core team facilitated the collaboration, multiple options valid</t>
+  </si>
+  <si>
+    <t>See [69] above</t>
+  </si>
+  <si>
+    <t>Open response to add context to [69] - [74] above. Varied interpretations, some redundant information.</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify H2H collaboration facilitation method</t>
+  </si>
+  <si>
+    <t>Check for how members engage with the network, multiple options valid</t>
+  </si>
+  <si>
+    <t>see [76] above</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify internal channel method</t>
+  </si>
+  <si>
+    <t>see [76] above, open response option</t>
+  </si>
+  <si>
+    <t>Very little information, remove</t>
+  </si>
+  <si>
+    <t>Open response for suggesting future programming; lots of unique information, but should be read in context unless H2H wants us to aggregate, but we should clarify what they are looking for</t>
+  </si>
+  <si>
+    <t>Remove for aggregation, but should check with H2H to see if there's some info they are looking for in these open responses</t>
+  </si>
+  <si>
+    <t>Open response for suggesting future member services, lots of unique information and suggestion that should be read in context</t>
+  </si>
+  <si>
+    <t>Yes/No for if member has applied to H2H fund</t>
+  </si>
+  <si>
+    <t>Open response for comment on [85] above. Most seem to be referencing specific funds they applied for but some varied interpretaion; H2H should read in context</t>
+  </si>
+  <si>
+    <t>Asking for the reason org did not aly to funding, multiple options valid</t>
+  </si>
+  <si>
+    <t>See [87] above</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify why funding not sought</t>
+  </si>
+  <si>
+    <t>See [87] above; open response. Not many responses, but should be read in context.</t>
+  </si>
+  <si>
+    <t>Yes/No check on if feedback from H2H when denied funding was useful</t>
+  </si>
+  <si>
+    <t>Open response comment on [97] above. Varied interpretation, lots of unique information that should be read in context.</t>
+  </si>
+  <si>
+    <t>5 point likert scale for perceived transparency in H2H decision making process</t>
+  </si>
+  <si>
+    <t>Rewrite header, load responses as is</t>
+  </si>
+  <si>
+    <t>Open response on [99] above, varied interpretation with a lot of overlap and reference to [98] above. Should be read in context.</t>
+  </si>
+  <si>
+    <t>5 point likert scale for support provided by H2H during the fund activation process</t>
+  </si>
+  <si>
+    <t>Open response on the future of the fund, lots of unique information worth reading in context.</t>
+  </si>
+  <si>
+    <t>Open response on [101] above, varied interpretation and lots of unique resposnes worth reading in context.</t>
+  </si>
+  <si>
+    <t>Yes/No for awareness of the network increasing over the last year</t>
+  </si>
+  <si>
+    <t>Open response on [104] above, varied interpretation. General sentiment seems to be "hard to say", but worth reading in context.</t>
+  </si>
+  <si>
+    <t>Open response for how org communicates to agencies, donors, and nationa lactiors about H2H. Varied interpretation but lots of unique info. Could categorize but need some guidance.</t>
+  </si>
+  <si>
+    <t>Ranked list for which activities H2H engages in support external engagement for the network, comma delimeted.</t>
+  </si>
+  <si>
+    <t>Create three columns one for each option in the list, and parse the responses into the columns with a score (1 for first in the list, 2 for second ,3 for third)</t>
+  </si>
+  <si>
+    <t>Open response on [107] above, not many responses here, some confusion about the question.</t>
+  </si>
+  <si>
+    <t>Question for which external channels the org uses to engage with the network, multipel options valid</t>
+  </si>
+  <si>
+    <t>See [109] above</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify external communication method</t>
+  </si>
+  <si>
+    <t>See [109] above; open response comments, all of them say email, so might be worth just collapsing this into an email option</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify external communication method is email, load as 1 or 0</t>
+  </si>
+  <si>
+    <t>Org perspective and what activities most effectively support external enagement, multiple options valid</t>
+  </si>
+  <si>
+    <t>See [115] above</t>
+  </si>
+  <si>
+    <t>Rewrite header to clarify activity around fund activations</t>
+  </si>
+  <si>
+    <t>See [115] above, open response comment. Very low response rate, better to just read in context.</t>
+  </si>
+  <si>
+    <t>Open response for suggestions on H2H's brokering and facilitation activities, very low response rate. Worth reading in context.</t>
+  </si>
+  <si>
+    <t>Time stamp for survey start</t>
+  </si>
+  <si>
+    <t>Time stamp for survey completion</t>
+  </si>
+  <si>
+    <t>Unique ID for respondant network</t>
+  </si>
+  <si>
+    <t>Empty column</t>
   </si>
 </sst>
 </file>
@@ -1703,15 +1853,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2032,15 +2182,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7FEF52-89A2-2F42-A286-59280B1D433F}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="70.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.83203125" customWidth="1"/>
@@ -2048,12 +2198,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5">
+      <c r="A1" s="8">
         <v>2019</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="9">
         <v>2023</v>
       </c>
@@ -2071,7 +2221,7 @@
       <c r="C2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>374</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -2097,7 +2247,7 @@
       <c r="C3" t="s">
         <v>356</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -2123,7 +2273,7 @@
       <c r="C4" t="s">
         <v>356</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -2149,7 +2299,7 @@
       <c r="C5" t="s">
         <v>356</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2175,7 +2325,7 @@
       <c r="C6" t="s">
         <v>356</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2201,7 +2351,7 @@
       <c r="C7" t="s">
         <v>356</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2227,7 +2377,7 @@
       <c r="C8" t="s">
         <v>356</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>445</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2253,7 +2403,7 @@
       <c r="C9" t="s">
         <v>356</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>446</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2279,7 +2429,7 @@
       <c r="C10" t="s">
         <v>356</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>446</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2305,7 +2455,7 @@
       <c r="C11" t="s">
         <v>356</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2331,7 +2481,7 @@
       <c r="C12" t="s">
         <v>367</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>375</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2357,7 +2507,7 @@
       <c r="C13" t="s">
         <v>369</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>376</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2383,7 +2533,7 @@
       <c r="C14" t="s">
         <v>356</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2409,7 +2559,7 @@
       <c r="C15" t="s">
         <v>356</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2435,7 +2585,7 @@
       <c r="C16" t="s">
         <v>356</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2461,7 +2611,7 @@
       <c r="C17" t="s">
         <v>356</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2487,7 +2637,7 @@
       <c r="C18" t="s">
         <v>356</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2513,7 +2663,7 @@
       <c r="C19" t="s">
         <v>356</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2539,7 +2689,7 @@
       <c r="C20" t="s">
         <v>356</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2565,7 +2715,7 @@
       <c r="C21" t="s">
         <v>356</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2591,7 +2741,7 @@
       <c r="C22" t="s">
         <v>356</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2617,7 +2767,7 @@
       <c r="C23" t="s">
         <v>356</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2643,7 +2793,7 @@
       <c r="C24" t="s">
         <v>356</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2669,7 +2819,7 @@
       <c r="C25" t="s">
         <v>356</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -2695,7 +2845,7 @@
       <c r="C26" t="s">
         <v>356</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2721,7 +2871,7 @@
       <c r="C27" t="s">
         <v>356</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2747,7 +2897,7 @@
       <c r="C28" t="s">
         <v>356</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2773,7 +2923,7 @@
       <c r="C29" t="s">
         <v>356</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -2799,7 +2949,7 @@
       <c r="C30" t="s">
         <v>356</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -2825,7 +2975,7 @@
       <c r="C31" t="s">
         <v>356</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2851,7 +3001,7 @@
       <c r="C32" t="s">
         <v>356</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -2877,7 +3027,7 @@
       <c r="C33" t="s">
         <v>356</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -2903,7 +3053,7 @@
       <c r="C34" t="s">
         <v>356</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -2929,7 +3079,7 @@
       <c r="C35" t="s">
         <v>356</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2955,7 +3105,7 @@
       <c r="C36" t="s">
         <v>356</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -2981,7 +3131,7 @@
       <c r="C37" t="s">
         <v>356</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -3007,7 +3157,7 @@
       <c r="C38" t="s">
         <v>356</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -3033,7 +3183,7 @@
       <c r="C39" t="s">
         <v>356</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -3059,7 +3209,7 @@
       <c r="C40" t="s">
         <v>356</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -3085,7 +3235,7 @@
       <c r="C41" t="s">
         <v>356</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3111,7 +3261,7 @@
       <c r="C42" t="s">
         <v>356</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3137,7 +3287,7 @@
       <c r="C43" t="s">
         <v>356</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -3163,7 +3313,7 @@
       <c r="C44" t="s">
         <v>356</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -3189,7 +3339,7 @@
       <c r="C45" t="s">
         <v>356</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3215,7 +3365,7 @@
       <c r="C46" t="s">
         <v>356</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3241,7 +3391,7 @@
       <c r="C47" t="s">
         <v>356</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3267,7 +3417,7 @@
       <c r="C48" t="s">
         <v>356</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3293,7 +3443,7 @@
       <c r="C49" t="s">
         <v>356</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -3319,7 +3469,7 @@
       <c r="C50" t="s">
         <v>356</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3345,7 +3495,7 @@
       <c r="C51" t="s">
         <v>367</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>450</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -3371,7 +3521,7 @@
       <c r="C52" t="s">
         <v>384</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="6" t="s">
         <v>388</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -3397,7 +3547,7 @@
       <c r="C53" t="s">
         <v>385</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="6" t="s">
         <v>388</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -3423,7 +3573,7 @@
       <c r="C54" t="s">
         <v>390</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>389</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -3449,7 +3599,7 @@
       <c r="C55" t="s">
         <v>390</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="6" t="s">
         <v>389</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -3475,7 +3625,7 @@
       <c r="C56" t="s">
         <v>392</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -3501,7 +3651,7 @@
       <c r="C57" t="s">
         <v>392</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -3527,7 +3677,7 @@
       <c r="C58" t="s">
         <v>392</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -3553,7 +3703,7 @@
       <c r="C59" t="s">
         <v>392</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -3579,7 +3729,7 @@
       <c r="C60" t="s">
         <v>392</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -3605,7 +3755,7 @@
       <c r="C61" t="s">
         <v>392</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -3631,7 +3781,7 @@
       <c r="C62" t="s">
         <v>392</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -3657,7 +3807,7 @@
       <c r="C63" t="s">
         <v>392</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -3683,7 +3833,7 @@
       <c r="C64" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="6" t="s">
         <v>472</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -3709,7 +3859,7 @@
       <c r="C65" t="s">
         <v>392</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -3735,7 +3885,7 @@
       <c r="C66" t="s">
         <v>392</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -3751,7 +3901,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -3761,17 +3911,23 @@
       <c r="C67" t="s">
         <v>392</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>292</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="H67" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -3781,17 +3937,23 @@
       <c r="C68" t="s">
         <v>392</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>293</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="H68" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -3801,17 +3963,23 @@
       <c r="C69" t="s">
         <v>392</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>294</v>
       </c>
+      <c r="F69" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="H69" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -3821,17 +3989,23 @@
       <c r="C70" t="s">
         <v>392</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>295</v>
       </c>
+      <c r="F70" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="H70" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -3841,17 +4015,23 @@
       <c r="C71" t="s">
         <v>392</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>296</v>
       </c>
+      <c r="F71" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>532</v>
+      </c>
       <c r="H71" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -3861,17 +4041,23 @@
       <c r="C72" t="s">
         <v>392</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>297</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>532</v>
+      </c>
       <c r="H72" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -3881,11 +4067,17 @@
       <c r="C73" t="s">
         <v>356</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>298</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>513</v>
@@ -3901,11 +4093,17 @@
       <c r="C74" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="6" t="s">
         <v>476</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>299</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>513</v>
@@ -3921,11 +4119,17 @@
       <c r="C75" t="s">
         <v>367</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="6" t="s">
         <v>483</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>300</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>513</v>
@@ -3941,17 +4145,23 @@
       <c r="C76" t="s">
         <v>484</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="F76" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>532</v>
+      </c>
       <c r="H76" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
@@ -3961,11 +4171,17 @@
       <c r="C77" t="s">
         <v>485</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="6" t="s">
         <v>482</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>302</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>513</v>
@@ -3981,17 +4197,23 @@
       <c r="C78" t="s">
         <v>406</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="F78" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="H78" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
@@ -4001,17 +4223,23 @@
       <c r="C79" t="s">
         <v>406</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="F79" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="H79" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -4021,17 +4249,23 @@
       <c r="C80" t="s">
         <v>406</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="F80" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="H80" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -4041,17 +4275,23 @@
       <c r="C81" t="s">
         <v>406</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="H81" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
@@ -4061,17 +4301,23 @@
       <c r="C82" t="s">
         <v>406</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="H82" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -4081,11 +4327,17 @@
       <c r="C83" t="s">
         <v>406</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="6" t="s">
         <v>489</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>308</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>535</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>513</v>
@@ -4101,17 +4353,23 @@
       <c r="C84" t="s">
         <v>407</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="6" t="s">
         <v>498</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="F84" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>537</v>
+      </c>
       <c r="H84" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -4121,17 +4379,23 @@
       <c r="C85" t="s">
         <v>407</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="6" t="s">
         <v>498</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>310</v>
       </c>
+      <c r="F85" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H85" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
@@ -4141,11 +4405,17 @@
       <c r="C86" t="s">
         <v>407</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="6" t="s">
         <v>498</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>311</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>513</v>
@@ -4161,17 +4431,23 @@
       <c r="C87" t="s">
         <v>356</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="6" t="s">
         <v>499</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>312</v>
       </c>
+      <c r="F87" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="H87" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -4181,11 +4457,17 @@
       <c r="C88" t="s">
         <v>367</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>313</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>513</v>
@@ -4201,11 +4483,17 @@
       <c r="C89" t="s">
         <v>356</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>314</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>513</v>
@@ -4221,11 +4509,17 @@
       <c r="C90" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D90" s="7" t="s">
         <v>503</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>315</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>513</v>
@@ -4241,11 +4535,17 @@
       <c r="C91" t="s">
         <v>356</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D91" s="7" t="s">
         <v>503</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>316</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>513</v>
@@ -4261,11 +4561,17 @@
       <c r="C92" t="s">
         <v>367</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>317</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>513</v>
@@ -4281,11 +4587,17 @@
       <c r="C93" t="s">
         <v>356</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>318</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>513</v>
@@ -4301,17 +4613,23 @@
       <c r="C94" t="s">
         <v>419</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>319</v>
       </c>
+      <c r="F94" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="H94" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -4321,17 +4639,23 @@
       <c r="C95" t="s">
         <v>419</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>320</v>
       </c>
+      <c r="F95" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="H95" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
@@ -4341,17 +4665,23 @@
       <c r="C96" t="s">
         <v>419</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>321</v>
       </c>
+      <c r="F96" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="H96" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
@@ -4361,17 +4691,23 @@
       <c r="C97" t="s">
         <v>419</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>322</v>
       </c>
+      <c r="F97" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="H97" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -4381,17 +4717,23 @@
       <c r="C98" t="s">
         <v>419</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>323</v>
       </c>
+      <c r="F98" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H98" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>96</v>
       </c>
@@ -4401,17 +4743,23 @@
       <c r="C99" t="s">
         <v>419</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>324</v>
       </c>
+      <c r="F99" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="H99" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>97</v>
       </c>
@@ -4421,17 +4769,23 @@
       <c r="C100" t="s">
         <v>419</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="F100" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H100" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
@@ -4441,17 +4795,23 @@
       <c r="C101" t="s">
         <v>419</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>326</v>
       </c>
+      <c r="F101" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>550</v>
+      </c>
       <c r="H101" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
@@ -4461,11 +4821,17 @@
       <c r="C102" t="s">
         <v>419</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="D102" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>327</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>513</v>
@@ -4481,11 +4847,17 @@
       <c r="C103" t="s">
         <v>356</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D103" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>328</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>550</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>513</v>
@@ -4501,17 +4873,23 @@
       <c r="C104" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D104" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="F104" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H104" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
@@ -4521,17 +4899,23 @@
       <c r="C105" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D105" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>330</v>
       </c>
+      <c r="F105" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H105" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>103</v>
       </c>
@@ -4541,17 +4925,23 @@
       <c r="C106" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="D106" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="F106" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="H106" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>104</v>
       </c>
@@ -4561,17 +4951,23 @@
       <c r="C107" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D107" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="F107" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H107" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>105</v>
       </c>
@@ -4581,17 +4977,23 @@
       <c r="C108" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="D108" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>333</v>
       </c>
+      <c r="F108" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H108" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>106</v>
       </c>
@@ -4601,11 +5003,17 @@
       <c r="C109" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D109" s="7" t="s">
+      <c r="D109" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>334</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>559</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>513</v>
@@ -4621,17 +5029,23 @@
       <c r="C110" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D110" s="7" t="s">
+      <c r="D110" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>335</v>
       </c>
+      <c r="F110" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>539</v>
+      </c>
       <c r="H110" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>108</v>
       </c>
@@ -4641,17 +5055,23 @@
       <c r="C111" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="D111" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>336</v>
       </c>
+      <c r="F111" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>563</v>
+      </c>
       <c r="H111" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>109</v>
       </c>
@@ -4661,17 +5081,23 @@
       <c r="C112" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D112" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>337</v>
       </c>
+      <c r="F112" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>563</v>
+      </c>
       <c r="H112" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>110</v>
       </c>
@@ -4681,17 +5107,23 @@
       <c r="C113" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>338</v>
       </c>
+      <c r="F113" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>563</v>
+      </c>
       <c r="H113" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>111</v>
       </c>
@@ -4701,11 +5133,17 @@
       <c r="C114" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="D114" s="6" t="s">
         <v>438</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>339</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>563</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>513</v>
@@ -4721,11 +5159,17 @@
       <c r="C115" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="D115" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>340</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>563</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>513</v>
@@ -4741,11 +5185,17 @@
       <c r="C116" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D116" s="8" t="s">
+      <c r="D116" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>341</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>513</v>
@@ -4761,11 +5211,17 @@
       <c r="C117" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="D117" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>342</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>513</v>
@@ -4781,11 +5237,17 @@
       <c r="C118" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D118" s="8" t="s">
+      <c r="D118" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>343</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>513</v>
@@ -4801,11 +5263,17 @@
       <c r="C119" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D119" s="8" t="s">
+      <c r="D119" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>344</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>513</v>
@@ -4821,11 +5289,17 @@
       <c r="C120" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D120" s="8" t="s">
+      <c r="D120" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>345</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>513</v>
@@ -4841,11 +5315,17 @@
       <c r="C121" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D121" s="8" t="s">
+      <c r="D121" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>346</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>513</v>
@@ -4861,11 +5341,17 @@
       <c r="C122" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D122" s="8" t="s">
+      <c r="D122" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>347</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>513</v>
@@ -4881,11 +5367,17 @@
       <c r="C123" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D123" s="8" t="s">
+      <c r="D123" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>348</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>513</v>
@@ -4901,11 +5393,17 @@
       <c r="C124" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D124" s="8" t="s">
+      <c r="D124" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>349</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>513</v>
@@ -4921,11 +5419,17 @@
       <c r="C125" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D125" s="8" t="s">
+      <c r="D125" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>350</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>513</v>
@@ -4941,11 +5445,17 @@
       <c r="C126" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D126" s="8" t="s">
+      <c r="D126" s="7" t="s">
         <v>507</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>351</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>513</v>
@@ -4961,7 +5471,7 @@
       <c r="C127" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D127" s="8" t="s">
+      <c r="D127" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4975,7 +5485,7 @@
       <c r="C128" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D128" s="8" t="s">
+      <c r="D128" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4989,7 +5499,7 @@
       <c r="C129" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D129" s="8" t="s">
+      <c r="D129" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5003,7 +5513,7 @@
       <c r="C130" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D130" s="8" t="s">
+      <c r="D130" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5017,7 +5527,7 @@
       <c r="C131" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="D131" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5031,7 +5541,7 @@
       <c r="C132" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D132" s="8" t="s">
+      <c r="D132" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5045,7 +5555,7 @@
       <c r="C133" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D133" s="8" t="s">
+      <c r="D133" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5059,7 +5569,7 @@
       <c r="C134" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D134" s="8" t="s">
+      <c r="D134" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5073,7 +5583,7 @@
       <c r="C135" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D135" s="8" t="s">
+      <c r="D135" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5087,7 +5597,7 @@
       <c r="C136" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D136" s="8" t="s">
+      <c r="D136" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5101,7 +5611,7 @@
       <c r="C137" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D137" s="8" t="s">
+      <c r="D137" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5115,7 +5625,7 @@
       <c r="C138" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D138" s="8" t="s">
+      <c r="D138" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5129,7 +5639,7 @@
       <c r="C139" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D139" s="8" t="s">
+      <c r="D139" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5143,7 +5653,7 @@
       <c r="C140" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D140" s="8" t="s">
+      <c r="D140" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5157,7 +5667,7 @@
       <c r="C141" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D141" s="8" t="s">
+      <c r="D141" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5171,7 +5681,7 @@
       <c r="C142" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D142" s="8" t="s">
+      <c r="D142" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5185,7 +5695,7 @@
       <c r="C143" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D143" s="8" t="s">
+      <c r="D143" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5199,7 +5709,7 @@
       <c r="C144" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D144" s="8" t="s">
+      <c r="D144" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5213,7 +5723,7 @@
       <c r="C145" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D145" s="8" t="s">
+      <c r="D145" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5227,7 +5737,7 @@
       <c r="C146" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D146" s="8" t="s">
+      <c r="D146" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5241,7 +5751,7 @@
       <c r="C147" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="D147" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5255,7 +5765,7 @@
       <c r="C148" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D148" s="8" t="s">
+      <c r="D148" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5269,7 +5779,7 @@
       <c r="C149" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D149" s="8" t="s">
+      <c r="D149" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5283,7 +5793,7 @@
       <c r="C150" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D150" s="8" t="s">
+      <c r="D150" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5297,7 +5807,7 @@
       <c r="C151" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D151" s="8" t="s">
+      <c r="D151" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5311,7 +5821,7 @@
       <c r="C152" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D152" s="8" t="s">
+      <c r="D152" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5325,7 +5835,7 @@
       <c r="C153" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D153" s="8" t="s">
+      <c r="D153" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5339,7 +5849,7 @@
       <c r="C154" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D154" s="8" t="s">
+      <c r="D154" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5353,7 +5863,7 @@
       <c r="C155" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D155" s="8" t="s">
+      <c r="D155" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5367,7 +5877,7 @@
       <c r="C156" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D156" s="8" t="s">
+      <c r="D156" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5381,7 +5891,7 @@
       <c r="C157" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D157" s="8" t="s">
+      <c r="D157" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5395,7 +5905,7 @@
       <c r="C158" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D158" s="8" t="s">
+      <c r="D158" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5409,7 +5919,7 @@
       <c r="C159" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D159" s="8" t="s">
+      <c r="D159" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5423,7 +5933,7 @@
       <c r="C160" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D160" s="8" t="s">
+      <c r="D160" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5437,7 +5947,7 @@
       <c r="C161" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="D161" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5451,7 +5961,7 @@
       <c r="C162" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D162" s="8" t="s">
+      <c r="D162" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5465,7 +5975,7 @@
       <c r="C163" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D163" s="8" t="s">
+      <c r="D163" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5479,7 +5989,7 @@
       <c r="C164" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D164" s="8" t="s">
+      <c r="D164" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5493,7 +6003,7 @@
       <c r="C165" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D165" s="8" t="s">
+      <c r="D165" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5507,7 +6017,7 @@
       <c r="C166" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D166" s="8" t="s">
+      <c r="D166" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5521,7 +6031,7 @@
       <c r="C167" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D167" s="8" t="s">
+      <c r="D167" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5535,7 +6045,7 @@
       <c r="C168" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D168" s="8" t="s">
+      <c r="D168" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5549,7 +6059,7 @@
       <c r="C169" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D169" s="8" t="s">
+      <c r="D169" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5563,7 +6073,7 @@
       <c r="C170" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D170" s="8" t="s">
+      <c r="D170" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5577,7 +6087,7 @@
       <c r="C171" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D171" s="8" t="s">
+      <c r="D171" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5591,7 +6101,7 @@
       <c r="C172" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D172" s="8" t="s">
+      <c r="D172" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5605,7 +6115,7 @@
       <c r="C173" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D173" s="8" t="s">
+      <c r="D173" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5619,7 +6129,7 @@
       <c r="C174" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D174" s="8" t="s">
+      <c r="D174" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5633,7 +6143,7 @@
       <c r="C175" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D175" s="8" t="s">
+      <c r="D175" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5647,7 +6157,7 @@
       <c r="C176" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D176" s="8" t="s">
+      <c r="D176" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5661,7 +6171,7 @@
       <c r="C177" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D177" s="8" t="s">
+      <c r="D177" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5675,7 +6185,7 @@
       <c r="C178" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D178" s="8" t="s">
+      <c r="D178" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5689,7 +6199,7 @@
       <c r="C179" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D179" s="8" t="s">
+      <c r="D179" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5703,7 +6213,7 @@
       <c r="C180" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D180" s="8" t="s">
+      <c r="D180" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5717,7 +6227,7 @@
       <c r="C181" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D181" s="8" t="s">
+      <c r="D181" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5731,7 +6241,7 @@
       <c r="C182" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D182" s="8" t="s">
+      <c r="D182" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5745,7 +6255,7 @@
       <c r="C183" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D183" s="8" t="s">
+      <c r="D183" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5759,7 +6269,7 @@
       <c r="C184" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D184" s="8" t="s">
+      <c r="D184" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5773,7 +6283,7 @@
       <c r="C185" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D185" s="8" t="s">
+      <c r="D185" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5787,7 +6297,7 @@
       <c r="C186" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D186" s="8" t="s">
+      <c r="D186" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5801,7 +6311,7 @@
       <c r="C187" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D187" s="8" t="s">
+      <c r="D187" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5815,7 +6325,7 @@
       <c r="C188" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D188" s="8" t="s">
+      <c r="D188" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5829,7 +6339,7 @@
       <c r="C189" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D189" s="8" t="s">
+      <c r="D189" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5843,7 +6353,7 @@
       <c r="C190" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D190" s="8" t="s">
+      <c r="D190" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5857,7 +6367,7 @@
       <c r="C191" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D191" s="8" t="s">
+      <c r="D191" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5871,7 +6381,7 @@
       <c r="C192" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D192" s="8" t="s">
+      <c r="D192" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5885,7 +6395,7 @@
       <c r="C193" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D193" s="8" t="s">
+      <c r="D193" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5899,7 +6409,7 @@
       <c r="C194" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D194" s="8" t="s">
+      <c r="D194" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5913,7 +6423,7 @@
       <c r="C195" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D195" s="8" t="s">
+      <c r="D195" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5927,7 +6437,7 @@
       <c r="C196" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D196" s="8" t="s">
+      <c r="D196" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5941,7 +6451,7 @@
       <c r="C197" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D197" s="8" t="s">
+      <c r="D197" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5955,7 +6465,7 @@
       <c r="C198" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D198" s="8" t="s">
+      <c r="D198" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5969,7 +6479,7 @@
       <c r="C199" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D199" s="8" t="s">
+      <c r="D199" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5983,7 +6493,7 @@
       <c r="C200" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D200" s="8" t="s">
+      <c r="D200" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5997,7 +6507,7 @@
       <c r="C201" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D201" s="8" t="s">
+      <c r="D201" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6011,7 +6521,7 @@
       <c r="C202" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D202" s="8" t="s">
+      <c r="D202" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6025,7 +6535,7 @@
       <c r="C203" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D203" s="8" t="s">
+      <c r="D203" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6039,7 +6549,7 @@
       <c r="C204" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D204" s="8" t="s">
+      <c r="D204" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6053,7 +6563,7 @@
       <c r="C205" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D205" s="8" t="s">
+      <c r="D205" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6067,7 +6577,7 @@
       <c r="C206" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D206" s="8" t="s">
+      <c r="D206" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6081,7 +6591,7 @@
       <c r="C207" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D207" s="8" t="s">
+      <c r="D207" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6095,7 +6605,7 @@
       <c r="C208" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D208" s="8" t="s">
+      <c r="D208" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6109,7 +6619,7 @@
       <c r="C209" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D209" s="8" t="s">
+      <c r="D209" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6123,7 +6633,7 @@
       <c r="C210" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D210" s="8" t="s">
+      <c r="D210" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6137,7 +6647,7 @@
       <c r="C211" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D211" s="8" t="s">
+      <c r="D211" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6151,7 +6661,7 @@
       <c r="C212" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D212" s="8" t="s">
+      <c r="D212" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6165,7 +6675,7 @@
       <c r="C213" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D213" s="8" t="s">
+      <c r="D213" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6179,7 +6689,7 @@
       <c r="C214" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D214" s="8" t="s">
+      <c r="D214" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6193,7 +6703,7 @@
       <c r="C215" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D215" s="8" t="s">
+      <c r="D215" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6207,7 +6717,7 @@
       <c r="C216" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D216" s="8" t="s">
+      <c r="D216" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6221,7 +6731,7 @@
       <c r="C217" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D217" s="8" t="s">
+      <c r="D217" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6235,7 +6745,7 @@
       <c r="C218" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D218" s="8" t="s">
+      <c r="D218" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6249,7 +6759,7 @@
       <c r="C219" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D219" s="8" t="s">
+      <c r="D219" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6263,7 +6773,7 @@
       <c r="C220" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D220" s="8" t="s">
+      <c r="D220" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6277,7 +6787,7 @@
       <c r="C221" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D221" s="8" t="s">
+      <c r="D221" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6291,7 +6801,7 @@
       <c r="C222" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D222" s="8" t="s">
+      <c r="D222" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6305,7 +6815,7 @@
       <c r="C223" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D223" s="8" t="s">
+      <c r="D223" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6319,7 +6829,7 @@
       <c r="C224" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D224" s="8" t="s">
+      <c r="D224" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6333,7 +6843,7 @@
       <c r="C225" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D225" s="8" t="s">
+      <c r="D225" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6347,7 +6857,7 @@
       <c r="C226" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D226" s="8" t="s">
+      <c r="D226" s="7" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6361,7 +6871,7 @@
       <c r="C227" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D227" s="8" t="s">
+      <c r="D227" s="7" t="s">
         <v>511</v>
       </c>
     </row>
@@ -6375,7 +6885,7 @@
       <c r="C228" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D228" s="8" t="s">
+      <c r="D228" s="7" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6389,7 +6899,7 @@
       <c r="C229" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="D229" s="8" t="s">
+      <c r="D229" s="7" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6403,7 +6913,7 @@
       <c r="C230" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D230" s="8" t="s">
+      <c r="D230" s="7" t="s">
         <v>438</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added export of current clean csvs
</commit_message>
<xml_diff>
--- a/docs/Data Cleanup Procedure Breakdown.xlsx
+++ b/docs/Data Cleanup Procedure Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812C591-EBC6-5041-B3B0-B904098E1060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227950C0-0CDA-2E45-B1EB-9628FA7DBC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="7240" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
+    <workbookView xWindow="1700" yWindow="3500" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="926">
   <si>
     <t xml:space="preserve">[1] "Respondent ID"                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
   </si>
@@ -2448,6 +2448,372 @@
   </si>
   <si>
     <t>Q30_Org_Public_Description_Open_Response</t>
+  </si>
+  <si>
+    <t>PII_Response_ID</t>
+  </si>
+  <si>
+    <t>Q03_PII_Respondent_Name</t>
+  </si>
+  <si>
+    <t>Q04_PII_Respondent_Email</t>
+  </si>
+  <si>
+    <t>Q05_PII_Respondent_Phone</t>
+  </si>
+  <si>
+    <t>Q06_Org_Year_Founded</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Ind_NGO</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Hosted_Proj</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Foundation</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Commercial_Ent</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Social_Ent</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Other</t>
+  </si>
+  <si>
+    <t>Q07_Org_Type_Open_Response</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_0_200000</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_200001_500000</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_500001_2000000</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_2000001_5000000</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_5000001_10000000</t>
+  </si>
+  <si>
+    <t>Q08_Org_Revenue_1000000_Plus</t>
+  </si>
+  <si>
+    <t>Q09_Percent_H2H_Work_Open_Response</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Inst_Donor</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Sub_Grant</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Foundations</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Membership_Fees</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Funds</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Commercial</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Other</t>
+  </si>
+  <si>
+    <t>Q10_Funding_Source_Open_Response</t>
+  </si>
+  <si>
+    <t>Q11_Insitutional_Donors</t>
+  </si>
+  <si>
+    <t>Q11_Insitutional_Donors_Open_Response</t>
+  </si>
+  <si>
+    <t>Q12_Num_Paid_Employees_Open_Response</t>
+  </si>
+  <si>
+    <t>Q13_Num_Volunteers_Open_Response</t>
+  </si>
+  <si>
+    <t>Q14_Grants_Received_None</t>
+  </si>
+  <si>
+    <t>Q14_Grants_Received_Range_10000_100000</t>
+  </si>
+  <si>
+    <t>Q14_Grants_Received_Range_100001_250000</t>
+  </si>
+  <si>
+    <t>Q14_Grants_Received_Range_250001_500000</t>
+  </si>
+  <si>
+    <t>Q14_Grants_Received_Range_500001_Plus</t>
+  </si>
+  <si>
+    <t>Q15_Org_Deploy_To_Crisis</t>
+  </si>
+  <si>
+    <t>Q15_Org_Deploy_To_Crisis_Open_Response</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_Global</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_Europe</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_API</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_Latin_America</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_Middle_East</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_West_Central_Africa</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_Southern_Eastern_Africa</t>
+  </si>
+  <si>
+    <t>Q16_Org_Geographic_Projects_None</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_Donors</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_UN_Agencies</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_Red_Cross</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_International_NGO</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_Local_National_Org</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_Other</t>
+  </si>
+  <si>
+    <t>Q17_Org_End_User_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ01_H2H_Network_Satisfaction</t>
+  </si>
+  <si>
+    <t>SQ01_H2H_Network_Satisfaction_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Type_Board_Member</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Type_Calls_Workshops</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Type_Community_Of_Practice</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Type_Network_Events</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ02_Level_Involvement_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ03_Collaborated_With_Other_H2H_Member</t>
+  </si>
+  <si>
+    <t>SQ03_Collaborated_With_Other_H2H_Member_Type_Formal</t>
+  </si>
+  <si>
+    <t>SQ03_Collaborated_With_Other_H2H_Member_Type_Informal</t>
+  </si>
+  <si>
+    <t>SQ03_Collaborated_With_Other_H2H_Member_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Fund_Activation</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Community_Of_Practice</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Events</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Webinars</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Not_Applicable</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ04_H2H_Facilitated_Collab_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Calls_Emails</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Monthly_Updates</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Sharepoint</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Slack</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Crisis_Watch_Calls</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ05_Network_Engagement_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ06_Community_Of_Practice_Suggestions_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ07_Member_Services_Suggestions_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ08_Applied_For_H2H_Fund</t>
+  </si>
+  <si>
+    <t>SQ08_Applied_For_H2H_Fund_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Unclear_Process</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Misaligned_Priorities_Capacities</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Alternate_Funding</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Submission_Timeframe_Short</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Complex_Process</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Due_Dilligence_Assessment</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Amount_Small</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Implment_Timeframe_Short</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ09_Avoided_H2H_Fund_Reason_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ10_H2H_Fund_Rejection_Feedback_Useful</t>
+  </si>
+  <si>
+    <t>SQ10_H2H_Fund_Rejection_Feedback_Useful_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ11_Grant_Panel_Assessment_Decision_Process</t>
+  </si>
+  <si>
+    <t>SQ11_Grant_Panel_Assessment_Decision_Process_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ12_Grant_Support_Provided</t>
+  </si>
+  <si>
+    <t>SQ12_Grant_Support_Provided_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ13_Fund_Development_Suggestions_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ14_Greater_Awareness_Of_Network</t>
+  </si>
+  <si>
+    <t>SQ14_Greater_Awareness_Of_Network_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ15_How_Communicate_About_H2H</t>
+  </si>
+  <si>
+    <t>SQ16_Rank_External_Engagement_Approach</t>
+  </si>
+  <si>
+    <t>SQ16_Rank_External_Engagement_Approach_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Type_Social_Media</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Type_Website</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Type_Newsletter</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Type_Events</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ17_External_Network_Engagement_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ18_Fund_Activation_External_Enagagement_Type_Comms_Package</t>
+  </si>
+  <si>
+    <t>SQ18_Fund_Activation_External_Enagagement_Type_Stakeholder_Brokering</t>
+  </si>
+  <si>
+    <t>SQ18_Fund_Activation_External_Enagagement_Type_Deployment</t>
+  </si>
+  <si>
+    <t>SQ18_Fund_Activation_External_Enagagement_Type_Other</t>
+  </si>
+  <si>
+    <t>SQ18_Fund_Activation_External_Enagagement_Open_Response</t>
+  </si>
+  <si>
+    <t>SQ19_H2H_Brokering_Facilitation_Suggestions_Open_Response</t>
+  </si>
+  <si>
+    <t>PII_Survey_Start</t>
+  </si>
+  <si>
+    <t>PII_Survey_Finish</t>
+  </si>
+  <si>
+    <t>PII_Network_ID</t>
+  </si>
+  <si>
+    <t>PII_Empty_Tags</t>
   </si>
 </sst>
 </file>
@@ -2867,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7FEF52-89A2-2F42-A286-59280B1D433F}">
-  <dimension ref="A1:I230"/>
+  <dimension ref="A1:J230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2878,13 +3244,13 @@
     <col min="1" max="2" width="60.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="45.6640625" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="70.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.83203125" customWidth="1"/>
-    <col min="9" max="9" width="44" customWidth="1"/>
+    <col min="6" max="7" width="70.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+    <col min="10" max="10" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8">
         <v>2019</v>
       </c>
@@ -2898,8 +3264,9 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>352</v>
       </c>
@@ -2919,16 +3286,19 @@
         <v>352</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2948,16 +3318,19 @@
         <v>228</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>356</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2977,16 +3350,19 @@
         <v>229</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>367</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3006,16 +3382,19 @@
         <v>230</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>369</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3035,16 +3414,19 @@
         <v>231</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>356</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3064,16 +3446,19 @@
         <v>232</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>356</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3093,16 +3478,19 @@
         <v>233</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>356</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3122,16 +3510,19 @@
         <v>234</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3151,16 +3542,19 @@
         <v>235</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>452</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3180,16 +3574,19 @@
         <v>236</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>452</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -3209,16 +3606,19 @@
         <v>237</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>452</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -3238,16 +3638,19 @@
         <v>238</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>452</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -3267,16 +3670,19 @@
         <v>239</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>452</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3296,16 +3702,19 @@
         <v>240</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3325,16 +3734,19 @@
         <v>241</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3354,16 +3766,19 @@
         <v>242</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3383,16 +3798,19 @@
         <v>243</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3412,16 +3830,19 @@
         <v>244</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3441,16 +3862,19 @@
         <v>245</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3470,16 +3894,19 @@
         <v>246</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3499,16 +3926,19 @@
         <v>247</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3528,16 +3958,19 @@
         <v>248</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3557,16 +3990,19 @@
         <v>249</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3586,16 +4022,19 @@
         <v>250</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -3615,16 +4054,19 @@
         <v>251</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -3644,16 +4086,19 @@
         <v>252</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3673,16 +4118,19 @@
         <v>253</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -3702,16 +4150,19 @@
         <v>254</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -3731,16 +4182,19 @@
         <v>255</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -3760,16 +4214,19 @@
         <v>256</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -3789,16 +4246,19 @@
         <v>257</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -3818,16 +4278,19 @@
         <v>258</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -3847,16 +4310,19 @@
         <v>259</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -3876,16 +4342,19 @@
         <v>260</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -3905,16 +4374,19 @@
         <v>261</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -3934,16 +4406,19 @@
         <v>262</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3963,16 +4438,19 @@
         <v>263</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -3992,16 +4470,19 @@
         <v>264</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -4021,16 +4502,19 @@
         <v>265</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -4050,16 +4534,19 @@
         <v>266</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -4079,16 +4566,19 @@
         <v>267</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -4108,16 +4598,19 @@
         <v>268</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -4137,16 +4630,19 @@
         <v>269</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -4166,16 +4662,19 @@
         <v>270</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -4195,16 +4694,19 @@
         <v>271</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -4224,16 +4726,19 @@
         <v>272</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -4253,16 +4758,19 @@
         <v>273</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -4282,16 +4790,19 @@
         <v>274</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -4311,16 +4822,19 @@
         <v>275</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -4340,16 +4854,19 @@
         <v>276</v>
       </c>
       <c r="G51" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4369,16 +4886,19 @@
         <v>277</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -4398,16 +4918,19 @@
         <v>278</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -4427,16 +4950,19 @@
         <v>279</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -4456,16 +4982,19 @@
         <v>280</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -4485,16 +5014,19 @@
         <v>281</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -4514,16 +5046,19 @@
         <v>282</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -4543,16 +5078,19 @@
         <v>283</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -4572,16 +5110,19 @@
         <v>284</v>
       </c>
       <c r="G59" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -4601,16 +5142,19 @@
         <v>285</v>
       </c>
       <c r="G60" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="I60" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -4630,16 +5174,19 @@
         <v>286</v>
       </c>
       <c r="G61" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="I61" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -4659,16 +5206,19 @@
         <v>287</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -4688,16 +5238,19 @@
         <v>288</v>
       </c>
       <c r="G63" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="I63" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -4717,16 +5270,19 @@
         <v>289</v>
       </c>
       <c r="G64" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="I64" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -4746,16 +5302,19 @@
         <v>290</v>
       </c>
       <c r="G65" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="I65" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -4775,16 +5334,19 @@
         <v>291</v>
       </c>
       <c r="G66" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="I66" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -4804,16 +5366,19 @@
         <v>292</v>
       </c>
       <c r="G67" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="I67" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -4833,16 +5398,19 @@
         <v>293</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I68" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="J68" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -4862,16 +5430,19 @@
         <v>294</v>
       </c>
       <c r="G69" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -4891,16 +5462,19 @@
         <v>295</v>
       </c>
       <c r="G70" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -4920,16 +5494,19 @@
         <v>296</v>
       </c>
       <c r="G71" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="I71" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -4949,16 +5526,19 @@
         <v>297</v>
       </c>
       <c r="G72" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="I72" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="J72" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -4978,16 +5558,19 @@
         <v>298</v>
       </c>
       <c r="G73" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="I73" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
@@ -5007,16 +5590,19 @@
         <v>299</v>
       </c>
       <c r="G74" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="I74" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
@@ -5036,16 +5622,19 @@
         <v>300</v>
       </c>
       <c r="G75" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="H75" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="I75" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
@@ -5065,16 +5654,19 @@
         <v>301</v>
       </c>
       <c r="G76" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
@@ -5094,16 +5686,19 @@
         <v>302</v>
       </c>
       <c r="G77" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="H77" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="I77" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I77" s="1" t="s">
+      <c r="J77" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -5123,16 +5718,19 @@
         <v>303</v>
       </c>
       <c r="G78" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="I78" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I78" s="1" t="s">
+      <c r="J78" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
@@ -5152,16 +5750,19 @@
         <v>304</v>
       </c>
       <c r="G79" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="I79" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="J79" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -5181,16 +5782,19 @@
         <v>305</v>
       </c>
       <c r="G80" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="I80" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="J80" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -5210,16 +5814,19 @@
         <v>306</v>
       </c>
       <c r="G81" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="H81" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H81" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I81" s="1" t="s">
+      <c r="J81" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
@@ -5239,16 +5846,19 @@
         <v>307</v>
       </c>
       <c r="G82" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I82" s="1" t="s">
+      <c r="J82" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -5268,16 +5878,19 @@
         <v>308</v>
       </c>
       <c r="G83" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="I83" s="1" t="s">
+      <c r="J83" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
@@ -5297,16 +5910,19 @@
         <v>309</v>
       </c>
       <c r="G84" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="I84" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="I84" s="1" t="s">
+      <c r="J84" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -5326,16 +5942,19 @@
         <v>310</v>
       </c>
       <c r="G85" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="H85" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="H85" s="1" t="s">
+      <c r="I85" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I85" s="1" t="s">
+      <c r="J85" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
@@ -5355,16 +5974,19 @@
         <v>311</v>
       </c>
       <c r="G86" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="H86" s="1" t="s">
+      <c r="I86" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I86" s="1" t="s">
+      <c r="J86" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
@@ -5384,16 +6006,19 @@
         <v>312</v>
       </c>
       <c r="G87" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="H87" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="H87" s="1" t="s">
+      <c r="I87" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="J87" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -5413,16 +6038,19 @@
         <v>313</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="I88" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I88" s="1" t="s">
+      <c r="J88" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
@@ -5442,16 +6070,19 @@
         <v>314</v>
       </c>
       <c r="G89" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="H89" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="H89" s="1" t="s">
+      <c r="I89" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I89" s="1" t="s">
+      <c r="J89" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -5471,16 +6102,19 @@
         <v>315</v>
       </c>
       <c r="G90" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="H90" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H90" s="1" t="s">
+      <c r="I90" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="J90" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
@@ -5500,16 +6134,19 @@
         <v>316</v>
       </c>
       <c r="G91" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="I91" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I91" s="1" t="s">
+      <c r="J91" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
@@ -5529,16 +6166,19 @@
         <v>317</v>
       </c>
       <c r="G92" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="I92" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I92" s="1" t="s">
+      <c r="J92" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -5558,16 +6198,19 @@
         <v>318</v>
       </c>
       <c r="G93" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="H93" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H93" s="1" t="s">
+      <c r="I93" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I93" s="1" t="s">
+      <c r="J93" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -5587,16 +6230,19 @@
         <v>319</v>
       </c>
       <c r="G94" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="H94" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I94" s="1" t="s">
+      <c r="J94" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -5616,16 +6262,19 @@
         <v>320</v>
       </c>
       <c r="G95" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="H95" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H95" s="1" t="s">
+      <c r="I95" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I95" s="1" t="s">
+      <c r="J95" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
@@ -5645,16 +6294,19 @@
         <v>321</v>
       </c>
       <c r="G96" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="H96" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="I96" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I96" s="1" t="s">
+      <c r="J96" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
@@ -5674,16 +6326,19 @@
         <v>322</v>
       </c>
       <c r="G97" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="H97" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H97" s="1" t="s">
+      <c r="I97" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I97" s="1" t="s">
+      <c r="J97" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -5703,16 +6358,19 @@
         <v>323</v>
       </c>
       <c r="G98" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="H98" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="H98" s="1" t="s">
+      <c r="I98" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I98" s="1" t="s">
+      <c r="J98" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>96</v>
       </c>
@@ -5732,16 +6390,19 @@
         <v>324</v>
       </c>
       <c r="G99" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="I99" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="I99" s="1" t="s">
+      <c r="J99" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>97</v>
       </c>
@@ -5761,16 +6422,19 @@
         <v>325</v>
       </c>
       <c r="G100" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="H100" s="1" t="s">
+      <c r="I100" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I100" s="1" t="s">
+      <c r="J100" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
@@ -5790,16 +6454,19 @@
         <v>326</v>
       </c>
       <c r="G101" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="H101" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="H101" s="1" t="s">
+      <c r="I101" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="I101" s="1" t="s">
+      <c r="J101" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
@@ -5819,16 +6486,19 @@
         <v>327</v>
       </c>
       <c r="G102" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="H102" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="H102" s="1" t="s">
+      <c r="I102" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I102" s="1" t="s">
+      <c r="J102" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
@@ -5848,16 +6518,19 @@
         <v>328</v>
       </c>
       <c r="G103" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="H103" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="H103" s="1" t="s">
+      <c r="I103" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="I103" s="1" t="s">
+      <c r="J103" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>101</v>
       </c>
@@ -5877,16 +6550,19 @@
         <v>329</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="H104" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="I104" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="J104" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
@@ -5906,16 +6582,19 @@
         <v>330</v>
       </c>
       <c r="G105" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="H105" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="I105" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I105" s="1" t="s">
+      <c r="J105" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>103</v>
       </c>
@@ -5935,16 +6614,19 @@
         <v>331</v>
       </c>
       <c r="G106" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="H106" s="1" t="s">
+      <c r="I106" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="I106" s="1" t="s">
+      <c r="J106" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>104</v>
       </c>
@@ -5964,16 +6646,19 @@
         <v>332</v>
       </c>
       <c r="G107" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="I107" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I107" s="1" t="s">
+      <c r="J107" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>105</v>
       </c>
@@ -5993,16 +6678,19 @@
         <v>333</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="I108" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I108" s="1" t="s">
+      <c r="J108" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>106</v>
       </c>
@@ -6022,16 +6710,19 @@
         <v>334</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="H109" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="H109" s="1" t="s">
+      <c r="I109" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="I109" s="1" t="s">
+      <c r="J109" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" ht="136" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>107</v>
       </c>
@@ -6051,16 +6742,19 @@
         <v>335</v>
       </c>
       <c r="G110" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="H110" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="I110" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I110" s="1" t="s">
+      <c r="J110" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>108</v>
       </c>
@@ -6080,16 +6774,19 @@
         <v>336</v>
       </c>
       <c r="G111" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="H111" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="H111" s="1" t="s">
+      <c r="I111" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="I111" s="1" t="s">
+      <c r="J111" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>109</v>
       </c>
@@ -6109,16 +6806,19 @@
         <v>337</v>
       </c>
       <c r="G112" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="H112" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="H112" s="1" t="s">
+      <c r="I112" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="I112" s="1" t="s">
+      <c r="J112" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>110</v>
       </c>
@@ -6138,16 +6838,19 @@
         <v>338</v>
       </c>
       <c r="G113" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="H113" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="H113" s="1" t="s">
+      <c r="I113" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="I113" s="1" t="s">
+      <c r="J113" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>111</v>
       </c>
@@ -6167,16 +6870,19 @@
         <v>339</v>
       </c>
       <c r="G114" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="H114" s="1" t="s">
+      <c r="I114" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="I114" s="1" t="s">
+      <c r="J114" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>112</v>
       </c>
@@ -6196,16 +6902,19 @@
         <v>340</v>
       </c>
       <c r="G115" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="H115" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="I115" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="I115" s="1" t="s">
+      <c r="J115" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>113</v>
       </c>
@@ -6225,16 +6934,19 @@
         <v>341</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="H116" s="1" t="s">
+      <c r="I116" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="I116" s="1" t="s">
+      <c r="J116" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>114</v>
       </c>
@@ -6254,16 +6966,19 @@
         <v>342</v>
       </c>
       <c r="G117" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="I117" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="I117" s="1" t="s">
+      <c r="J117" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>115</v>
       </c>
@@ -6283,16 +6998,19 @@
         <v>343</v>
       </c>
       <c r="G118" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="H118" s="1" t="s">
+      <c r="I118" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="I118" s="1" t="s">
+      <c r="J118" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>116</v>
       </c>
@@ -6312,16 +7030,19 @@
         <v>344</v>
       </c>
       <c r="G119" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="H119" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="H119" s="1" t="s">
+      <c r="I119" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="I119" s="1" t="s">
+      <c r="J119" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>117</v>
       </c>
@@ -6341,16 +7062,19 @@
         <v>345</v>
       </c>
       <c r="G120" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="H120" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="H120" s="1" t="s">
+      <c r="I120" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="I120" s="1" t="s">
+      <c r="J120" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>118</v>
       </c>
@@ -6370,16 +7094,19 @@
         <v>346</v>
       </c>
       <c r="G121" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="H121" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="H121" s="1" t="s">
+      <c r="I121" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I121" s="1" t="s">
+      <c r="J121" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>119</v>
       </c>
@@ -6399,16 +7126,19 @@
         <v>347</v>
       </c>
       <c r="G122" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="H122" s="1" t="s">
+      <c r="I122" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I122" s="1" t="s">
+      <c r="J122" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>120</v>
       </c>
@@ -6428,16 +7158,19 @@
         <v>348</v>
       </c>
       <c r="G123" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="H123" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="H123" s="1" t="s">
+      <c r="I123" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I123" s="1" t="s">
+      <c r="J123" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>121</v>
       </c>
@@ -6457,16 +7190,19 @@
         <v>349</v>
       </c>
       <c r="G124" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="H124" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="H124" s="1" t="s">
+      <c r="I124" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I124" s="1" t="s">
+      <c r="J124" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>122</v>
       </c>
@@ -6486,16 +7222,19 @@
         <v>350</v>
       </c>
       <c r="G125" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="H125" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="H125" s="1" t="s">
+      <c r="I125" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I125" s="1" t="s">
+      <c r="J125" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>123</v>
       </c>
@@ -6515,16 +7254,19 @@
         <v>351</v>
       </c>
       <c r="G126" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="H126" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="H126" s="1" t="s">
+      <c r="I126" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I126" s="1" t="s">
+      <c r="J126" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>124</v>
       </c>
@@ -6541,7 +7283,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>125</v>
       </c>
@@ -8295,7 +9037,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 2023 to 2019 data map to docs
</commit_message>
<xml_diff>
--- a/docs/Data Cleanup Procedure Breakdown.xlsx
+++ b/docs/Data Cleanup Procedure Breakdown.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia/My Drive/Projects/Statistics Without Borders/SWB-231 H2H/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227950C0-0CDA-2E45-B1EB-9628FA7DBC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECC7C7-D729-064C-9C8F-FF4A96B441A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="3500" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="34560" windowHeight="21100" xr2:uid="{9070B722-F9D2-0B4C-9C85-DE161E51A2BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7FEF52-89A2-2F42-A286-59280B1D433F}">
   <dimension ref="A1:J230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G126"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>